<commit_message>
update tables post fix function
</commit_message>
<xml_diff>
--- a/output/tables/comp_tab.xlsx
+++ b/output/tables/comp_tab.xlsx
@@ -377,7 +377,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>㥌FI = 0; ΔRMSEA = 0.</t>
+          <t>ΔCFI = 0; ΔRMSEA = 0.</t>
         </is>
       </c>
     </row>
@@ -389,7 +389,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>㥌FI = 0; ΔRMSEA = 0.</t>
+          <t>ΔCFI = 0; ΔRMSEA = 0.</t>
         </is>
       </c>
     </row>
@@ -401,7 +401,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>㥌FI = 0; ΔRMSEA = 0.</t>
+          <t>ΔCFI = 0; ΔRMSEA = 0.</t>
         </is>
       </c>
     </row>
@@ -413,7 +413,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>㥌FI = 0; ΔRMSEA = 0.</t>
+          <t>ΔCFI = 0; ΔRMSEA = 0.</t>
         </is>
       </c>
     </row>
@@ -425,7 +425,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>㥌FI = 0; ΔRMSEA = 0.</t>
+          <t>ΔCFI = 0; ΔRMSEA = 0.01.</t>
         </is>
       </c>
     </row>
@@ -437,7 +437,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>㥌FI = 0; ΔRMSEA = 0.01.</t>
+          <t>ΔCFI = 0; ΔRMSEA = 0.</t>
         </is>
       </c>
     </row>
@@ -449,7 +449,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>㥌FI = 0; ΔRMSEA = 0.</t>
+          <t>ΔCFI = 0; ΔRMSEA = 0.</t>
         </is>
       </c>
     </row>
@@ -461,7 +461,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>㥌FI = 0; ΔRMSEA = 0.</t>
+          <t>ΔCFI = 0; ΔRMSEA = 0.</t>
         </is>
       </c>
     </row>
@@ -473,7 +473,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>㥌FI = 0; ΔRMSEA = 0.</t>
+          <t>ΔCFI = 0; ΔRMSEA = 0.</t>
         </is>
       </c>
     </row>

</xml_diff>